<commit_message>
Updated estimated effort xls
</commit_message>
<xml_diff>
--- a/FCBI_Estimated_Effort.xlsx
+++ b/FCBI_Estimated_Effort.xlsx
@@ -406,7 +406,7 @@
     <t>Alex, James T</t>
   </si>
   <si>
-    <t>Unit Testing</t>
+    <t>Manual Testing</t>
   </si>
   <si>
     <r>
@@ -1116,7 +1116,7 @@
       <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="6" fillId="5" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" shrinkToFit="0" vertical="center" wrapText="1"/>
+      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="6" fillId="5" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
@@ -2586,7 +2586,7 @@
       <c r="H21" s="77"/>
       <c r="I21" s="41">
         <f>SUM(H22:H30)</f>
-        <v>69</v>
+        <v>134</v>
       </c>
       <c r="J21" s="5"/>
       <c r="K21" s="5"/>
@@ -2893,7 +2893,7 @@
       </c>
       <c r="G26" s="83"/>
       <c r="H26" s="88">
-        <v>0.0</v>
+        <v>25.0</v>
       </c>
       <c r="I26" s="83"/>
       <c r="J26" s="4"/>
@@ -2904,7 +2904,7 @@
         <v>0</v>
       </c>
       <c r="N26" s="89">
-        <v>0.0</v>
+        <v>15.0</v>
       </c>
       <c r="O26" s="53">
         <f t="shared" si="20"/>
@@ -2915,7 +2915,7 @@
         <v>0</v>
       </c>
       <c r="Q26" s="89">
-        <v>0.0</v>
+        <v>10.0</v>
       </c>
       <c r="R26" s="55">
         <f t="shared" si="23"/>
@@ -2923,7 +2923,7 @@
       </c>
       <c r="S26" s="55">
         <f t="shared" si="24"/>
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="T26" s="4"/>
       <c r="U26" s="4"/>
@@ -2956,14 +2956,14 @@
       </c>
       <c r="G27" s="83"/>
       <c r="H27" s="88">
-        <v>0.0</v>
+        <v>3.0</v>
       </c>
       <c r="I27" s="83"/>
       <c r="J27" s="4"/>
       <c r="K27" s="4"/>
       <c r="L27" s="4"/>
       <c r="M27" s="90">
-        <v>0.0</v>
+        <v>3.0</v>
       </c>
       <c r="N27" s="55">
         <f>IF(ISNUMBER(FIND($N$2,$E27)),$F27,0)</f>
@@ -2987,7 +2987,7 @@
       </c>
       <c r="S27" s="55">
         <f t="shared" si="24"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="T27" s="4"/>
       <c r="U27" s="4"/>
@@ -3020,7 +3020,7 @@
       </c>
       <c r="G28" s="83"/>
       <c r="H28" s="88">
-        <v>0.0</v>
+        <v>10.0</v>
       </c>
       <c r="I28" s="83"/>
       <c r="J28" s="4"/>
@@ -3031,7 +3031,7 @@
         <v>0</v>
       </c>
       <c r="N28" s="89">
-        <v>0.0</v>
+        <v>10.0</v>
       </c>
       <c r="O28" s="53">
         <f t="shared" si="20"/>
@@ -3051,7 +3051,7 @@
       </c>
       <c r="S28" s="55">
         <f t="shared" si="24"/>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="T28" s="4"/>
       <c r="U28" s="4"/>
@@ -3084,7 +3084,7 @@
       </c>
       <c r="G29" s="96"/>
       <c r="H29" s="95">
-        <v>3.0</v>
+        <v>20.0</v>
       </c>
       <c r="I29" s="96"/>
       <c r="J29" s="4"/>
@@ -3142,7 +3142,7 @@
       </c>
       <c r="G30" s="108"/>
       <c r="H30" s="109">
-        <v>0.0</v>
+        <v>10.0</v>
       </c>
       <c r="I30" s="108"/>
       <c r="J30" s="4"/>
@@ -3157,10 +3157,10 @@
         <v>0</v>
       </c>
       <c r="O30" s="111">
-        <v>0.0</v>
+        <v>5.0</v>
       </c>
       <c r="P30" s="90">
-        <v>0.0</v>
+        <v>5.0</v>
       </c>
       <c r="Q30" s="55">
         <f>IF(ISNUMBER(FIND($Q$2,$E30)),$F30,0)</f>
@@ -3172,7 +3172,7 @@
       </c>
       <c r="S30" s="112">
         <f>SUM(M30:R30)</f>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="T30" s="4"/>
       <c r="U30" s="4"/>
@@ -3204,7 +3204,7 @@
       <c r="H31" s="115"/>
       <c r="I31" s="40">
         <f>SUM(H32:H34)</f>
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="J31" s="4"/>
       <c r="K31" s="4"/>
@@ -3247,7 +3247,7 @@
       </c>
       <c r="G32" s="83"/>
       <c r="H32" s="88">
-        <v>0.0</v>
+        <v>10.0</v>
       </c>
       <c r="I32" s="83"/>
       <c r="J32" s="4"/>
@@ -3262,10 +3262,10 @@
         <v>0</v>
       </c>
       <c r="O32" s="111">
-        <v>0.0</v>
+        <v>5.0</v>
       </c>
       <c r="P32" s="117">
-        <v>0.0</v>
+        <v>5.0</v>
       </c>
       <c r="Q32" s="54">
         <f t="shared" ref="Q32:Q34" si="27">IF(ISNUMBER(FIND($Q$2,$E32)),$F32,0)</f>
@@ -3309,14 +3309,14 @@
       </c>
       <c r="G33" s="83"/>
       <c r="H33" s="88">
-        <v>0.0</v>
+        <v>15.0</v>
       </c>
       <c r="I33" s="83"/>
       <c r="J33" s="4"/>
       <c r="K33" s="4"/>
       <c r="L33" s="4"/>
       <c r="M33" s="117">
-        <v>0.0</v>
+        <v>5.0</v>
       </c>
       <c r="N33" s="116">
         <f t="shared" si="26"/>
@@ -3335,7 +3335,7 @@
         <v>0</v>
       </c>
       <c r="R33" s="111">
-        <v>0.0</v>
+        <v>10.0</v>
       </c>
       <c r="S33" s="117">
         <v>0.0</v>
@@ -3371,7 +3371,7 @@
       </c>
       <c r="G34" s="83"/>
       <c r="H34" s="88">
-        <v>0.0</v>
+        <v>5.0</v>
       </c>
       <c r="I34" s="83"/>
       <c r="J34" s="4"/>
@@ -3398,11 +3398,11 @@
         <v>0</v>
       </c>
       <c r="R34" s="111">
-        <v>0.0</v>
+        <v>5.0</v>
       </c>
       <c r="S34" s="116">
         <f t="shared" ref="S34:S35" si="32">SUM(M34:R34)</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="T34" s="4"/>
       <c r="U34" s="4"/>
@@ -3436,42 +3436,42 @@
       </c>
       <c r="H35" s="124">
         <f>SUM(M35:R35)</f>
-        <v>164</v>
+        <v>242</v>
       </c>
       <c r="I35" s="123">
         <f>SUM(I5:I34)</f>
-        <v>164</v>
+        <v>259</v>
       </c>
       <c r="J35" s="125"/>
       <c r="K35" s="125"/>
       <c r="L35" s="125"/>
       <c r="M35" s="124">
         <f t="shared" ref="M35:R35" si="31">SUM(M5:M34)</f>
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="N35" s="124">
         <f t="shared" si="31"/>
-        <v>22</v>
+        <v>47</v>
       </c>
       <c r="O35" s="124">
         <f t="shared" si="31"/>
-        <v>25</v>
+        <v>35</v>
       </c>
       <c r="P35" s="124">
         <f t="shared" si="31"/>
-        <v>25</v>
+        <v>35</v>
       </c>
       <c r="Q35" s="124">
         <f t="shared" si="31"/>
-        <v>36</v>
+        <v>46</v>
       </c>
       <c r="R35" s="124">
         <f t="shared" si="31"/>
-        <v>24</v>
+        <v>39</v>
       </c>
       <c r="S35" s="124">
         <f t="shared" si="32"/>
-        <v>164</v>
+        <v>242</v>
       </c>
       <c r="T35" s="1"/>
       <c r="U35" s="5"/>

</xml_diff>